<commit_message>
feat(upload): subida a bbdd de los datos del excel
</commit_message>
<xml_diff>
--- a/files/plantillas/Eventos_Plantilla.xlsx
+++ b/files/plantillas/Eventos_Plantilla.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TFG\files\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DBC58B-EE18-4B7A-A772-CC5434744D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B43A9F-21DC-4A31-B149-42A05F8F091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="2850" windowWidth="15375" windowHeight="7875" xr2:uid="{817DB277-A4FD-472E-8062-2E9A55FC1AC8}"/>
+    <workbookView xWindow="3360" yWindow="5340" windowWidth="14400" windowHeight="4800" xr2:uid="{817DB277-A4FD-472E-8062-2E9A55FC1AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>nombre</t>
   </si>
@@ -78,9 +72,6 @@
   </si>
   <si>
     <t>gratis</t>
-  </si>
-  <si>
-    <t>audiencia</t>
   </si>
   <si>
     <t>dias</t>
@@ -456,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821AF7D3-8B9E-4696-8484-C308FB63B4D4}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,12 +512,6 @@
       </c>
       <c r="S1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(plantillas): cambios en plantillas
</commit_message>
<xml_diff>
--- a/files/plantillas/Eventos_Plantilla.xlsx
+++ b/files/plantillas/Eventos_Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TFG\files\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B43A9F-21DC-4A31-B149-42A05F8F091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCD3F90-C676-46E8-B0D2-97D27A12ED6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="5340" windowWidth="14400" windowHeight="4800" xr2:uid="{817DB277-A4FD-472E-8062-2E9A55FC1AC8}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" xr2:uid="{817DB277-A4FD-472E-8062-2E9A55FC1AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,70 +33,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>desc_sitio</t>
-  </si>
-  <si>
-    <t>horario</t>
-  </si>
-  <si>
-    <t>transporte</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>direccion</t>
-  </si>
-  <si>
-    <t>codpostal</t>
-  </si>
-  <si>
-    <t>latitud</t>
-  </si>
-  <si>
-    <t>longitud</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>fecha_ini</t>
-  </si>
-  <si>
-    <t>gratis</t>
-  </si>
-  <si>
-    <t>dias</t>
-  </si>
-  <si>
-    <t>dias_ex</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>lugar</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>telefono</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Codigo Postal</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Fecha fin</t>
+  </si>
+  <si>
+    <t>Fecha inicio</t>
+  </si>
+  <si>
+    <t>Gratis</t>
+  </si>
+  <si>
+    <t>Días</t>
+  </si>
+  <si>
+    <t>Días excluidos</t>
+  </si>
+  <si>
+    <t>Lugar</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Categorías</t>
+  </si>
+  <si>
+    <t>Audiencia</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>Texto libre</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>http://www.madrid.es</t>
+  </si>
+  <si>
+    <t>2022-11-04 00:00:00.0</t>
+  </si>
+  <si>
+    <t>2022-11-04 23:59:00.0</t>
+  </si>
+  <si>
+    <t>Avenida castilla 81</t>
+  </si>
+  <si>
+    <t>L,M,X,J,V,S,D</t>
+  </si>
+  <si>
+    <t>9/11/2022;29/10/2022;</t>
+  </si>
+  <si>
+    <t>Cineteca Madrid</t>
+  </si>
+  <si>
+    <t>/contenido/actividades</t>
+  </si>
+  <si>
+    <t>/usuario/Familias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +139,47 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,14 +191,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,15 +534,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821AF7D3-8B9E-4696-8484-C308FB63B4D4}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="22.08984375" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" customWidth="1"/>
+    <col min="10" max="10" width="19.90625" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" customWidth="1"/>
+    <col min="13" max="13" width="13.36328125" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="25.6328125" customWidth="1"/>
+    <col min="17" max="17" width="17.6328125" customWidth="1"/>
+    <col min="18" max="18" width="20.81640625" customWidth="1"/>
+    <col min="19" max="19" width="16.08984375" customWidth="1"/>
+    <col min="20" max="20" width="23.54296875" customWidth="1"/>
+    <col min="22" max="22" width="12.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,58 +569,112 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="3">
+        <v>9400</v>
+      </c>
+      <c r="N2" s="3">
+        <v>4042802889001870</v>
+      </c>
+      <c r="O2" s="3">
+        <v>-3710182353581840</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="Q4" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{32447E58-A735-4F3E-ACE0-FCBF3345C435}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>